<commit_message>
weight system implemented, working on multiple schedules, alternatives and professor time management
</commit_message>
<xml_diff>
--- a/PythonScheduler/output1.xlsx
+++ b/PythonScheduler/output1.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="737" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="645" uniqueCount="155">
   <si>
     <t>Course</t>
   </si>
@@ -62,150 +62,150 @@
     <t>10:00:00</t>
   </si>
   <si>
+    <t>Public Policy 105</t>
+  </si>
+  <si>
+    <t>scheduled</t>
+  </si>
+  <si>
+    <t>CMSC 291</t>
+  </si>
+  <si>
+    <t>Continued Computer Science for Non-Majors</t>
+  </si>
+  <si>
+    <t>Staff</t>
+  </si>
+  <si>
+    <t>Mon/Wed</t>
+  </si>
+  <si>
+    <t>Information Technology 227</t>
+  </si>
+  <si>
+    <t>CMSC 341</t>
+  </si>
+  <si>
+    <t>Data Structures</t>
+  </si>
+  <si>
+    <t>Marron, Christopher</t>
+  </si>
+  <si>
+    <t>Engineering 122, Engineering 122A</t>
+  </si>
+  <si>
+    <t>CMSC 441</t>
+  </si>
+  <si>
+    <t>Sherman Hall 013</t>
+  </si>
+  <si>
+    <t>CMSC 201</t>
+  </si>
+  <si>
+    <t>Computer Science I</t>
+  </si>
+  <si>
+    <t>Hamilton, Eric</t>
+  </si>
+  <si>
+    <t>13:00:00</t>
+  </si>
+  <si>
+    <t>CMSC 202</t>
+  </si>
+  <si>
+    <t>Computer Science II</t>
+  </si>
+  <si>
+    <t>Dixon, Jeremy</t>
+  </si>
+  <si>
+    <t>CMSC 203</t>
+  </si>
+  <si>
+    <t>Discrete Structures</t>
+  </si>
+  <si>
+    <t>Joeg, Prasanna</t>
+  </si>
+  <si>
+    <t>CMSC 313</t>
+  </si>
+  <si>
+    <t>Comp. Org. &amp; Assembly Lang.</t>
+  </si>
+  <si>
+    <t>Kartchner, Jeannette</t>
+  </si>
+  <si>
+    <t>CMSC 331</t>
+  </si>
+  <si>
+    <t>Programming Languages</t>
+  </si>
+  <si>
+    <t>Donyaee, Kash</t>
+  </si>
+  <si>
+    <t>Janet &amp; Walter Sondheim 109</t>
+  </si>
+  <si>
+    <t>Johnson, Benjamin</t>
+  </si>
+  <si>
+    <t>Math &amp; Psychology 106</t>
+  </si>
+  <si>
+    <t>CMSC 411cs</t>
+  </si>
+  <si>
+    <t>Computer Architecture</t>
+  </si>
+  <si>
+    <t>Sekyonda, Ivan</t>
+  </si>
+  <si>
+    <t>Meyerhoff Chemistry 030</t>
+  </si>
+  <si>
+    <t>CMSC 435/634</t>
+  </si>
+  <si>
+    <t>Computer Graphics</t>
+  </si>
+  <si>
+    <t>Olano, Marc</t>
+  </si>
+  <si>
     <t>Sherman Hall 014</t>
   </si>
   <si>
-    <t>scheduled</t>
-  </si>
-  <si>
-    <t>CMSC 291</t>
-  </si>
-  <si>
-    <t>Continued Computer Science for Non-Majors</t>
-  </si>
-  <si>
-    <t>Staff</t>
-  </si>
-  <si>
-    <t>Mon/Wed</t>
-  </si>
-  <si>
-    <t>Information Technology 227</t>
-  </si>
-  <si>
-    <t>CMSC 341</t>
-  </si>
-  <si>
-    <t>Data Structures</t>
-  </si>
-  <si>
-    <t>Marron, Christopher</t>
+    <t>CMSC 447</t>
+  </si>
+  <si>
+    <t>Software Engineering I</t>
+  </si>
+  <si>
+    <t>Dutt, Abhijit</t>
+  </si>
+  <si>
+    <t>Sherman Hall 151</t>
+  </si>
+  <si>
+    <t>CMSC 476/676</t>
+  </si>
+  <si>
+    <t>Information Retrieval</t>
+  </si>
+  <si>
+    <t>Pearce, Claudia</t>
   </si>
   <si>
     <t>Interdisciplinary Life S 237</t>
   </si>
   <si>
-    <t>CMSC 441</t>
-  </si>
-  <si>
-    <t>Sherman Hall 013</t>
-  </si>
-  <si>
-    <t>CMSC 201</t>
-  </si>
-  <si>
-    <t>Computer Science I</t>
-  </si>
-  <si>
-    <t>Hamilton, Eric</t>
-  </si>
-  <si>
-    <t>13:00:00</t>
-  </si>
-  <si>
-    <t>Public Policy 105</t>
-  </si>
-  <si>
-    <t>CMSC 202</t>
-  </si>
-  <si>
-    <t>Computer Science II</t>
-  </si>
-  <si>
-    <t>Dixon, Jeremy</t>
-  </si>
-  <si>
-    <t>Engineering 122, Engineering 122A</t>
-  </si>
-  <si>
-    <t>CMSC 203</t>
-  </si>
-  <si>
-    <t>Discrete Structures</t>
-  </si>
-  <si>
-    <t>Joeg, Prasanna</t>
-  </si>
-  <si>
-    <t>CMSC 313</t>
-  </si>
-  <si>
-    <t>Comp. Org. &amp; Assembly Lang.</t>
-  </si>
-  <si>
-    <t>Kartchner, Jeannette</t>
-  </si>
-  <si>
-    <t>CMSC 331</t>
-  </si>
-  <si>
-    <t>Programming Languages</t>
-  </si>
-  <si>
-    <t>Donyaee, Kash</t>
-  </si>
-  <si>
-    <t>Johnson, Benjamin</t>
-  </si>
-  <si>
-    <t>Meyerhoff Chemistry 030</t>
-  </si>
-  <si>
-    <t>CMSC 411cs</t>
-  </si>
-  <si>
-    <t>Computer Architecture</t>
-  </si>
-  <si>
-    <t>Sekyonda, Ivan</t>
-  </si>
-  <si>
-    <t>Math &amp; Psychology 106</t>
-  </si>
-  <si>
-    <t>CMSC 435/634</t>
-  </si>
-  <si>
-    <t>Computer Graphics</t>
-  </si>
-  <si>
-    <t>Olano, Marc</t>
-  </si>
-  <si>
-    <t>CMSC 447</t>
-  </si>
-  <si>
-    <t>Software Engineering I</t>
-  </si>
-  <si>
-    <t>Dutt, Abhijit</t>
-  </si>
-  <si>
-    <t>Sherman Hall 151</t>
-  </si>
-  <si>
-    <t>CMSC 476/676</t>
-  </si>
-  <si>
-    <t>Information Retrieval</t>
-  </si>
-  <si>
-    <t>Pearce, Claudia</t>
-  </si>
-  <si>
-    <t>Janet &amp; Walter Sondheim 109</t>
-  </si>
-  <si>
     <t>CMSC 201ss</t>
   </si>
   <si>
@@ -221,18 +221,18 @@
     <t>Databases</t>
   </si>
   <si>
+    <t>CMSC 684</t>
+  </si>
+  <si>
+    <t>Wireless Sensor Networks</t>
+  </si>
+  <si>
+    <t>Younis, Mohamed</t>
+  </si>
+  <si>
     <t>Biological Sciences 120</t>
   </si>
   <si>
-    <t>CMSC 684</t>
-  </si>
-  <si>
-    <t>Wireless Sensor Networks</t>
-  </si>
-  <si>
-    <t>Younis, Mohamed</t>
-  </si>
-  <si>
     <t>16:00:00</t>
   </si>
   <si>
@@ -314,123 +314,126 @@
     <t>Tues/Thurs</t>
   </si>
   <si>
+    <t>Yesha, Yaacov</t>
+  </si>
+  <si>
+    <t>Chang, Richard</t>
+  </si>
+  <si>
+    <t>CMSC 443/652</t>
+  </si>
+  <si>
+    <t>Cryptography and Data Security</t>
+  </si>
+  <si>
+    <t>Zhang, Haibin</t>
+  </si>
+  <si>
+    <t>11:30:00</t>
+  </si>
+  <si>
+    <t>Kalpakis, Kostas</t>
+  </si>
+  <si>
+    <t>CMSC 478</t>
+  </si>
+  <si>
+    <t>Machine Learning</t>
+  </si>
+  <si>
+    <t>Wilson, Marcella</t>
+  </si>
+  <si>
+    <t>CMSC 426</t>
+  </si>
+  <si>
+    <t>Computer Security</t>
+  </si>
+  <si>
+    <t>CMSC 493</t>
+  </si>
+  <si>
+    <t>Games Capstone</t>
+  </si>
+  <si>
+    <t>staff</t>
+  </si>
+  <si>
+    <t>CMSC 621</t>
+  </si>
+  <si>
+    <t>CMSC 411ce</t>
+  </si>
+  <si>
+    <t>Perkins, Dmitri</t>
+  </si>
+  <si>
+    <t>CMSC 479/679</t>
+  </si>
+  <si>
+    <t>Introduction to Robotics</t>
+  </si>
+  <si>
+    <t>Matuszek, Cynthia</t>
+  </si>
+  <si>
+    <t>CMSC 678</t>
+  </si>
+  <si>
+    <t>Oates, Tim</t>
+  </si>
+  <si>
+    <t>Finin, Tim</t>
+  </si>
+  <si>
+    <t>CMSC 481</t>
+  </si>
+  <si>
+    <t>Computer Networks</t>
+  </si>
+  <si>
+    <t>Sidhu, Deepinder</t>
+  </si>
+  <si>
+    <t>Spec Topic: Computer Vision</t>
+  </si>
+  <si>
+    <t>h</t>
+  </si>
+  <si>
+    <t>Chapman, David</t>
+  </si>
+  <si>
+    <t>CMSC 611</t>
+  </si>
+  <si>
+    <t>Liu, Chenchen</t>
+  </si>
+  <si>
+    <t>CMSC 483/691</t>
+  </si>
+  <si>
+    <t>Parallel &amp; Distr. Processing</t>
+  </si>
+  <si>
+    <t>Simon, Tyler</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spec Topic: Quantum Security </t>
+  </si>
+  <si>
+    <t>CMSC 487/687</t>
+  </si>
+  <si>
+    <t>Network Security</t>
+  </si>
+  <si>
+    <t>Zieglar, Edward</t>
+  </si>
+  <si>
     <t>unscheduled</t>
   </si>
   <si>
-    <t>Wilson, Marcella</t>
-  </si>
-  <si>
-    <t>Yesha, Yaacov</t>
-  </si>
-  <si>
-    <t>CMSC 411ce</t>
-  </si>
-  <si>
-    <t>Perkins, Dmitri</t>
-  </si>
-  <si>
-    <t>CMSC 426</t>
-  </si>
-  <si>
-    <t>Computer Security</t>
-  </si>
-  <si>
-    <t>Chang, Richard</t>
-  </si>
-  <si>
-    <t>CMSC 443/652</t>
-  </si>
-  <si>
-    <t>Cryptography and Data Security</t>
-  </si>
-  <si>
-    <t>Zhang, Haibin</t>
-  </si>
-  <si>
-    <t>Kalpakis, Kostas</t>
-  </si>
-  <si>
-    <t>Finin, Tim</t>
-  </si>
-  <si>
-    <t>CMSC 478</t>
-  </si>
-  <si>
-    <t>Machine Learning</t>
-  </si>
-  <si>
-    <t>CMSC 479/679</t>
-  </si>
-  <si>
-    <t>Introduction to Robotics</t>
-  </si>
-  <si>
-    <t>Matuszek, Cynthia</t>
-  </si>
-  <si>
-    <t>CMSC 481</t>
-  </si>
-  <si>
-    <t>Computer Networks</t>
-  </si>
-  <si>
-    <t>Sidhu, Deepinder</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Spec Topic: Quantum Security </t>
-  </si>
-  <si>
-    <t>CMSC 483/691</t>
-  </si>
-  <si>
-    <t>Parallel &amp; Distr. Processing</t>
-  </si>
-  <si>
-    <t>Simon, Tyler</t>
-  </si>
-  <si>
-    <t>CMSC 487/687</t>
-  </si>
-  <si>
-    <t>Network Security</t>
-  </si>
-  <si>
-    <t>Zieglar, Edward</t>
-  </si>
-  <si>
-    <t>Spec Topic: Computer Vision</t>
-  </si>
-  <si>
-    <t>h</t>
-  </si>
-  <si>
-    <t>Chapman, David</t>
-  </si>
-  <si>
-    <t>CMSC 493</t>
-  </si>
-  <si>
-    <t>Games Capstone</t>
-  </si>
-  <si>
-    <t>staff</t>
-  </si>
-  <si>
-    <t>CMSC 611</t>
-  </si>
-  <si>
-    <t>Liu, Chenchen</t>
-  </si>
-  <si>
-    <t>CMSC 621</t>
-  </si>
-  <si>
-    <t>CMSC 678</t>
-  </si>
-  <si>
-    <t>Oates, Tim</t>
-  </si>
-  <si>
     <t>CMSC 682</t>
   </si>
   <si>
@@ -455,172 +458,22 @@
     <t>alt3</t>
   </si>
   <si>
-    <t>CMSC 104Problem Solving &amp; Prog.3Staff</t>
-  </si>
-  <si>
-    <t>{'mw530': Biological Sciences 120}</t>
-  </si>
-  <si>
-    <t>{'mw530': Interdisciplinary Life S 233}</t>
-  </si>
-  <si>
-    <t>{'mw530': Public Policy 105}</t>
-  </si>
-  <si>
-    <t>CMSC 201Computer Science I2Johnson, Benjamin</t>
-  </si>
-  <si>
-    <t>{'mw230': Engineering 122, Engineering 122A}</t>
+    <t>CMSC 611Computer Architecture2Staff</t>
+  </si>
+  <si>
+    <t>{'mw230': Sherman Hall 014}</t>
+  </si>
+  <si>
+    <t>{'mw230': Interdisciplinary Life S 237}</t>
   </si>
   <si>
     <t>{'mw230': Public Policy 105}</t>
   </si>
   <si>
-    <t>CMSC 202Computer Science II1Dixon, Jeremy</t>
-  </si>
-  <si>
-    <t>CMSC 202Computer Science II3Donyaee, Kash</t>
-  </si>
-  <si>
-    <t>CMSC 202Computer Science II4Donyaee, Kash</t>
-  </si>
-  <si>
-    <t>CMSC 203Discrete Structures1Wilson, Marcella</t>
-  </si>
-  <si>
-    <t>CMSC 203Discrete Structures2Staff</t>
-  </si>
-  <si>
-    <t>CMSC 203Discrete Structures4Yesha, Yaacov</t>
-  </si>
-  <si>
-    <t>CMSC 203Discrete Structures5Yesha, Yaacov</t>
-  </si>
-  <si>
-    <t>CMSC 304Social &amp; Ethical Issues in IT1Staff</t>
-  </si>
-  <si>
-    <t>CMSC 304Social &amp; Ethical Issues in IT2Staff</t>
-  </si>
-  <si>
-    <t>CMSC 304Social &amp; Ethical Issues in IT3Staff</t>
-  </si>
-  <si>
-    <t>CMSC 304Social &amp; Ethical Issues in IT6Staff</t>
-  </si>
-  <si>
-    <t>CMSC 313Comp. Org. &amp; Assembly Lang.1Sekyonda, Ivan</t>
-  </si>
-  <si>
-    <t>CMSC 313Comp. Org. &amp; Assembly Lang.2Sekyonda, Ivan</t>
-  </si>
-  <si>
-    <t>CMSC 331Programming Languages1Donyaee, Kash</t>
-  </si>
-  <si>
-    <t>CMSC 331Programming Languages2Vafaei, Fereydoon</t>
-  </si>
-  <si>
-    <t>CMSC 331Programming Languages4Vafaei, Fereydoon</t>
-  </si>
-  <si>
-    <t>CMSC 341Data Structures2Wilson, Marcella</t>
-  </si>
-  <si>
-    <t>CMSC 341Data Structures3Wilson, Marcella</t>
-  </si>
-  <si>
-    <t>CMSC 411ceComputer Architecture1Squire, Jon</t>
-  </si>
-  <si>
-    <t>CMSC 411csComputer Architecture3Staff</t>
-  </si>
-  <si>
-    <t>CMSC 421Operating Systems1Staff</t>
-  </si>
-  <si>
-    <t>CMSC 421Operating Systems2Perkins, Dmitri</t>
-  </si>
-  <si>
-    <t>CMSC 426Computer Security1Staff</t>
-  </si>
-  <si>
-    <t>CMSC 426Computer Security3Staff</t>
-  </si>
-  <si>
-    <t>CMSC 441Algorithms1Chang, Richard</t>
-  </si>
-  <si>
-    <t>CMSC 441Algorithms2Chang, Richard</t>
-  </si>
-  <si>
-    <t>CMSC 443/652Cryptography and Data Security1Zhang, Haibin</t>
-  </si>
-  <si>
-    <t>{'mw230': Janet &amp; Walter Sondheim 109}</t>
-  </si>
-  <si>
-    <t>CMSC 447Software Engineering I3Staff</t>
-  </si>
-  <si>
-    <t>{'mw530': Sherman Hall 151}</t>
-  </si>
-  <si>
-    <t>CMSC 447Software Engineering I4Staff</t>
-  </si>
-  <si>
-    <t>CMSC 461Databases1Kalpakis, Kostas</t>
-  </si>
-  <si>
-    <t>CMSC 471Artificial Intelligence2Finin, Tim</t>
-  </si>
-  <si>
-    <t>CMSC 478Machine Learning1Staff</t>
-  </si>
-  <si>
-    <t>CMSC 478Machine Learning2Vafaei, Fereydoon</t>
-  </si>
-  <si>
-    <t>CMSC 479/679Introduction to Robotics1Matuszek, Cynthia</t>
-  </si>
-  <si>
-    <t>CMSC 481Computer Networks1Sidhu, Deepinder</t>
-  </si>
-  <si>
-    <t>CMSC 691Spec Topic: Quantum Security 1Sidhu, Deepinder</t>
-  </si>
-  <si>
-    <t>CMSC 483/691Parallel &amp; Distr. Processing1Simon, Tyler</t>
-  </si>
-  <si>
-    <t>CMSC 487/687Network Security1Zieglar, Edward</t>
-  </si>
-  <si>
-    <t>CMSC 491/691Spec Topic: Computer Vision1Chapman, David</t>
-  </si>
-  <si>
-    <t>CMSC 493Games Capstone1staff</t>
-  </si>
-  <si>
-    <t>CMSC 611Computer Architecture1Liu, Chenchen</t>
-  </si>
-  <si>
-    <t>CMSC 611Computer Architecture2Staff</t>
-  </si>
-  <si>
-    <t>CMSC 621Operating Systems1Kalpakis, Kostas</t>
-  </si>
-  <si>
-    <t>CMSC 678Machine Learning1Oates, Tim</t>
-  </si>
-  <si>
     <t>CMSC 682Network Technologies1Staff</t>
   </si>
   <si>
     <t>CMSC 682Network Technologies2Sidhu, Deepinder</t>
-  </si>
-  <si>
-    <t>CMSC 684Wireless Sensor Networks2Staff</t>
   </si>
   <si>
     <t>CMSC 491/691Spec Topic: Data Driven Design of Autonmous Systems1Zhu, Ting</t>
@@ -1135,7 +988,7 @@
         <v>31</v>
       </c>
       <c r="I6" t="s">
-        <v>32</v>
+        <v>15</v>
       </c>
       <c r="J6" t="s">
         <v>16</v>
@@ -1143,16 +996,16 @@
     </row>
     <row r="7" spans="1:10">
       <c r="A7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" t="s">
         <v>33</v>
-      </c>
-      <c r="B7" t="s">
-        <v>34</v>
       </c>
       <c r="D7">
         <v>5</v>
       </c>
       <c r="E7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F7">
         <v>100</v>
@@ -1164,7 +1017,7 @@
         <v>31</v>
       </c>
       <c r="I7" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="J7" t="s">
         <v>16</v>
@@ -1172,16 +1025,16 @@
     </row>
     <row r="8" spans="1:10">
       <c r="A8" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B8" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D8">
         <v>6</v>
       </c>
       <c r="E8" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F8">
         <v>40</v>
@@ -1201,16 +1054,16 @@
     </row>
     <row r="9" spans="1:10">
       <c r="A9" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B9" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D9">
         <v>3</v>
       </c>
       <c r="E9" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F9">
         <v>40</v>
@@ -1222,7 +1075,7 @@
         <v>31</v>
       </c>
       <c r="I9" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="J9" t="s">
         <v>16</v>
@@ -1230,16 +1083,16 @@
     </row>
     <row r="10" spans="1:10">
       <c r="A10" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B10" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D10">
         <v>3</v>
       </c>
       <c r="E10" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F10">
         <v>40</v>
@@ -1251,7 +1104,7 @@
         <v>31</v>
       </c>
       <c r="I10" t="s">
-        <v>27</v>
+        <v>44</v>
       </c>
       <c r="J10" t="s">
         <v>16</v>
@@ -1268,7 +1121,7 @@
         <v>4</v>
       </c>
       <c r="E11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F11">
         <v>40</v>
@@ -1280,7 +1133,7 @@
         <v>31</v>
       </c>
       <c r="I11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J11" t="s">
         <v>16</v>
@@ -1288,16 +1141,16 @@
     </row>
     <row r="12" spans="1:10">
       <c r="A12" t="s">
+        <v>47</v>
+      </c>
+      <c r="B12" t="s">
         <v>48</v>
       </c>
-      <c r="B12" t="s">
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12" t="s">
         <v>49</v>
-      </c>
-      <c r="D12">
-        <v>1</v>
-      </c>
-      <c r="E12" t="s">
-        <v>50</v>
       </c>
       <c r="F12">
         <v>40</v>
@@ -1309,7 +1162,7 @@
         <v>31</v>
       </c>
       <c r="I12" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J12" t="s">
         <v>16</v>
@@ -1317,16 +1170,16 @@
     </row>
     <row r="13" spans="1:10">
       <c r="A13" t="s">
+        <v>51</v>
+      </c>
+      <c r="B13" t="s">
         <v>52</v>
       </c>
-      <c r="B13" t="s">
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13" t="s">
         <v>53</v>
-      </c>
-      <c r="D13">
-        <v>1</v>
-      </c>
-      <c r="E13" t="s">
-        <v>54</v>
       </c>
       <c r="F13">
         <v>50</v>
@@ -1338,7 +1191,7 @@
         <v>31</v>
       </c>
       <c r="I13" t="s">
-        <v>15</v>
+        <v>54</v>
       </c>
       <c r="J13" t="s">
         <v>16</v>
@@ -1433,16 +1286,16 @@
     </row>
     <row r="17" spans="1:10">
       <c r="A17" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B17" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D17">
         <v>7</v>
       </c>
       <c r="E17" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F17">
         <v>40</v>
@@ -1462,16 +1315,16 @@
     </row>
     <row r="18" spans="1:10">
       <c r="A18" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B18" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D18">
         <v>4</v>
       </c>
       <c r="E18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F18">
         <v>40</v>
@@ -1512,7 +1365,7 @@
         <v>64</v>
       </c>
       <c r="I19" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="J19" t="s">
         <v>16</v>
@@ -1520,16 +1373,16 @@
     </row>
     <row r="20" spans="1:10">
       <c r="A20" t="s">
+        <v>47</v>
+      </c>
+      <c r="B20" t="s">
         <v>48</v>
-      </c>
-      <c r="B20" t="s">
-        <v>49</v>
       </c>
       <c r="D20">
         <v>2</v>
       </c>
       <c r="E20" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F20">
         <v>40</v>
@@ -1541,7 +1394,7 @@
         <v>64</v>
       </c>
       <c r="I20" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="J20" t="s">
         <v>16</v>
@@ -1599,7 +1452,7 @@
         <v>64</v>
       </c>
       <c r="I22" t="s">
-        <v>68</v>
+        <v>50</v>
       </c>
       <c r="J22" t="s">
         <v>16</v>
@@ -1607,16 +1460,16 @@
     </row>
     <row r="23" spans="1:10">
       <c r="A23" t="s">
+        <v>68</v>
+      </c>
+      <c r="B23" t="s">
         <v>69</v>
       </c>
-      <c r="B23" t="s">
+      <c r="D23">
+        <v>1</v>
+      </c>
+      <c r="E23" t="s">
         <v>70</v>
-      </c>
-      <c r="D23">
-        <v>1</v>
-      </c>
-      <c r="E23" t="s">
-        <v>71</v>
       </c>
       <c r="F23">
         <v>40</v>
@@ -1628,7 +1481,7 @@
         <v>64</v>
       </c>
       <c r="I23" t="s">
-        <v>21</v>
+        <v>71</v>
       </c>
       <c r="J23" t="s">
         <v>16</v>
@@ -1657,7 +1510,7 @@
         <v>72</v>
       </c>
       <c r="I24" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="J24" t="s">
         <v>16</v>
@@ -1674,7 +1527,7 @@
         <v>6</v>
       </c>
       <c r="E25" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F25">
         <v>40</v>
@@ -1715,7 +1568,7 @@
         <v>72</v>
       </c>
       <c r="I26" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="J26" t="s">
         <v>16</v>
@@ -1744,7 +1597,7 @@
         <v>72</v>
       </c>
       <c r="I27" t="s">
-        <v>15</v>
+        <v>54</v>
       </c>
       <c r="J27" t="s">
         <v>16</v>
@@ -1776,7 +1629,7 @@
         <v>72</v>
       </c>
       <c r="I28" t="s">
-        <v>27</v>
+        <v>44</v>
       </c>
       <c r="J28" t="s">
         <v>16</v>
@@ -1808,7 +1661,7 @@
         <v>72</v>
       </c>
       <c r="I29" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="J29" t="s">
         <v>16</v>
@@ -1845,16 +1698,16 @@
     </row>
     <row r="31" spans="1:10">
       <c r="A31" t="s">
+        <v>32</v>
+      </c>
+      <c r="B31" t="s">
         <v>33</v>
-      </c>
-      <c r="B31" t="s">
-        <v>34</v>
       </c>
       <c r="D31">
         <v>2</v>
       </c>
       <c r="E31" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F31">
         <v>100</v>
@@ -1866,7 +1719,7 @@
         <v>88</v>
       </c>
       <c r="I31" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="J31" t="s">
         <v>16</v>
@@ -1874,10 +1727,10 @@
     </row>
     <row r="32" spans="1:10">
       <c r="A32" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B32" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D32">
         <v>3</v>
@@ -1895,7 +1748,7 @@
         <v>88</v>
       </c>
       <c r="I32" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="J32" t="s">
         <v>16</v>
@@ -1924,7 +1777,7 @@
         <v>88</v>
       </c>
       <c r="I33" t="s">
-        <v>27</v>
+        <v>44</v>
       </c>
       <c r="J33" t="s">
         <v>16</v>
@@ -1953,7 +1806,7 @@
         <v>88</v>
       </c>
       <c r="I34" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J34" t="s">
         <v>16</v>
@@ -1982,7 +1835,7 @@
         <v>88</v>
       </c>
       <c r="I35" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J35" t="s">
         <v>16</v>
@@ -2011,7 +1864,7 @@
         <v>88</v>
       </c>
       <c r="I36" t="s">
-        <v>15</v>
+        <v>54</v>
       </c>
       <c r="J36" t="s">
         <v>16</v>
@@ -2080,39 +1933,45 @@
     </row>
     <row r="39" spans="1:10">
       <c r="A39" t="s">
-        <v>86</v>
+        <v>32</v>
       </c>
       <c r="B39" t="s">
-        <v>87</v>
+        <v>33</v>
       </c>
       <c r="D39">
         <v>1</v>
       </c>
       <c r="E39" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="F39">
-        <v>40</v>
+        <v>100</v>
       </c>
       <c r="G39" t="s">
         <v>98</v>
       </c>
+      <c r="H39" t="s">
+        <v>14</v>
+      </c>
+      <c r="I39" t="s">
+        <v>25</v>
+      </c>
       <c r="J39" t="s">
-        <v>99</v>
+        <v>16</v>
       </c>
     </row>
     <row r="40" spans="1:10">
       <c r="A40" t="s">
-        <v>86</v>
+        <v>35</v>
       </c>
       <c r="B40" t="s">
-        <v>87</v>
+        <v>36</v>
       </c>
       <c r="D40">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E40" t="s">
-        <v>19</v>
+        <v>99</v>
       </c>
       <c r="F40">
         <v>40</v>
@@ -2120,88 +1979,112 @@
       <c r="G40" t="s">
         <v>98</v>
       </c>
+      <c r="H40" t="s">
+        <v>14</v>
+      </c>
+      <c r="I40" t="s">
+        <v>21</v>
+      </c>
       <c r="J40" t="s">
-        <v>99</v>
+        <v>16</v>
       </c>
     </row>
     <row r="41" spans="1:10">
       <c r="A41" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="B41" t="s">
-        <v>29</v>
+        <v>42</v>
       </c>
       <c r="D41">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E41" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="F41">
-        <v>100</v>
+        <v>40</v>
       </c>
       <c r="G41" t="s">
         <v>98</v>
       </c>
+      <c r="H41" t="s">
+        <v>14</v>
+      </c>
+      <c r="I41" t="s">
+        <v>27</v>
+      </c>
       <c r="J41" t="s">
-        <v>99</v>
+        <v>16</v>
       </c>
     </row>
     <row r="42" spans="1:10">
       <c r="A42" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="B42" t="s">
-        <v>34</v>
+        <v>11</v>
       </c>
       <c r="D42">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E42" t="s">
-        <v>35</v>
+        <v>100</v>
       </c>
       <c r="F42">
-        <v>100</v>
+        <v>40</v>
       </c>
       <c r="G42" t="s">
         <v>98</v>
       </c>
+      <c r="H42" t="s">
+        <v>14</v>
+      </c>
+      <c r="I42" t="s">
+        <v>44</v>
+      </c>
       <c r="J42" t="s">
-        <v>99</v>
+        <v>16</v>
       </c>
     </row>
     <row r="43" spans="1:10">
       <c r="A43" t="s">
-        <v>33</v>
+        <v>101</v>
       </c>
       <c r="B43" t="s">
-        <v>34</v>
+        <v>102</v>
       </c>
       <c r="D43">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E43" t="s">
-        <v>45</v>
+        <v>103</v>
       </c>
       <c r="F43">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="G43" t="s">
         <v>98</v>
       </c>
+      <c r="H43" t="s">
+        <v>14</v>
+      </c>
+      <c r="I43" t="s">
+        <v>54</v>
+      </c>
       <c r="J43" t="s">
-        <v>99</v>
+        <v>16</v>
       </c>
     </row>
     <row r="44" spans="1:10">
       <c r="A44" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B44" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="D44">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E44" t="s">
         <v>45</v>
@@ -2212,68 +2095,86 @@
       <c r="G44" t="s">
         <v>98</v>
       </c>
+      <c r="H44" t="s">
+        <v>104</v>
+      </c>
+      <c r="I44" t="s">
+        <v>25</v>
+      </c>
       <c r="J44" t="s">
-        <v>99</v>
+        <v>16</v>
       </c>
     </row>
     <row r="45" spans="1:10">
       <c r="A45" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B45" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D45">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E45" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F45">
-        <v>80</v>
+        <v>40</v>
       </c>
       <c r="G45" t="s">
         <v>98</v>
       </c>
+      <c r="H45" t="s">
+        <v>104</v>
+      </c>
+      <c r="I45" t="s">
+        <v>21</v>
+      </c>
       <c r="J45" t="s">
-        <v>99</v>
+        <v>16</v>
       </c>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B46" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D46">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E46" t="s">
-        <v>19</v>
+        <v>49</v>
       </c>
       <c r="F46">
-        <v>80</v>
+        <v>40</v>
       </c>
       <c r="G46" t="s">
         <v>98</v>
       </c>
+      <c r="H46" t="s">
+        <v>104</v>
+      </c>
+      <c r="I46" t="s">
+        <v>27</v>
+      </c>
       <c r="J46" t="s">
-        <v>99</v>
+        <v>16</v>
       </c>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" t="s">
-        <v>37</v>
+        <v>91</v>
       </c>
       <c r="B47" t="s">
-        <v>38</v>
+        <v>92</v>
       </c>
       <c r="D47">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E47" t="s">
-        <v>101</v>
+        <v>19</v>
       </c>
       <c r="F47">
         <v>40</v>
@@ -2281,22 +2182,28 @@
       <c r="G47" t="s">
         <v>98</v>
       </c>
+      <c r="H47" t="s">
+        <v>104</v>
+      </c>
+      <c r="I47" t="s">
+        <v>44</v>
+      </c>
       <c r="J47" t="s">
-        <v>99</v>
+        <v>16</v>
       </c>
     </row>
     <row r="48" spans="1:10">
       <c r="A48" t="s">
-        <v>37</v>
+        <v>66</v>
       </c>
       <c r="B48" t="s">
-        <v>38</v>
+        <v>67</v>
       </c>
       <c r="D48">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E48" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="F48">
         <v>40</v>
@@ -2304,45 +2211,57 @@
       <c r="G48" t="s">
         <v>98</v>
       </c>
+      <c r="H48" t="s">
+        <v>104</v>
+      </c>
+      <c r="I48" t="s">
+        <v>46</v>
+      </c>
       <c r="J48" t="s">
-        <v>99</v>
+        <v>16</v>
       </c>
     </row>
     <row r="49" spans="1:10">
       <c r="A49" t="s">
-        <v>89</v>
+        <v>106</v>
       </c>
       <c r="B49" t="s">
-        <v>90</v>
+        <v>107</v>
       </c>
       <c r="D49">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E49" t="s">
-        <v>19</v>
+        <v>78</v>
       </c>
       <c r="F49">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="G49" t="s">
         <v>98</v>
       </c>
+      <c r="H49" t="s">
+        <v>104</v>
+      </c>
+      <c r="I49" t="s">
+        <v>54</v>
+      </c>
       <c r="J49" t="s">
-        <v>99</v>
+        <v>16</v>
       </c>
     </row>
     <row r="50" spans="1:10">
       <c r="A50" t="s">
-        <v>89</v>
+        <v>41</v>
       </c>
       <c r="B50" t="s">
-        <v>90</v>
+        <v>42</v>
       </c>
       <c r="D50">
         <v>2</v>
       </c>
       <c r="E50" t="s">
-        <v>19</v>
+        <v>78</v>
       </c>
       <c r="F50">
         <v>40</v>
@@ -2350,22 +2269,28 @@
       <c r="G50" t="s">
         <v>98</v>
       </c>
+      <c r="H50" t="s">
+        <v>31</v>
+      </c>
+      <c r="I50" t="s">
+        <v>21</v>
+      </c>
       <c r="J50" t="s">
-        <v>99</v>
+        <v>16</v>
       </c>
     </row>
     <row r="51" spans="1:10">
       <c r="A51" t="s">
-        <v>89</v>
+        <v>22</v>
       </c>
       <c r="B51" t="s">
-        <v>90</v>
+        <v>23</v>
       </c>
       <c r="D51">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E51" t="s">
-        <v>19</v>
+        <v>108</v>
       </c>
       <c r="F51">
         <v>40</v>
@@ -2373,19 +2298,25 @@
       <c r="G51" t="s">
         <v>98</v>
       </c>
+      <c r="H51" t="s">
+        <v>31</v>
+      </c>
+      <c r="I51" t="s">
+        <v>25</v>
+      </c>
       <c r="J51" t="s">
-        <v>99</v>
+        <v>16</v>
       </c>
     </row>
     <row r="52" spans="1:10">
       <c r="A52" t="s">
-        <v>89</v>
+        <v>109</v>
       </c>
       <c r="B52" t="s">
-        <v>90</v>
+        <v>110</v>
       </c>
       <c r="D52">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E52" t="s">
         <v>19</v>
@@ -2396,22 +2327,28 @@
       <c r="G52" t="s">
         <v>98</v>
       </c>
+      <c r="H52" t="s">
+        <v>31</v>
+      </c>
+      <c r="I52" t="s">
+        <v>27</v>
+      </c>
       <c r="J52" t="s">
-        <v>99</v>
+        <v>16</v>
       </c>
     </row>
     <row r="53" spans="1:10">
       <c r="A53" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="B53" t="s">
-        <v>41</v>
+        <v>11</v>
       </c>
       <c r="D53">
         <v>1</v>
       </c>
       <c r="E53" t="s">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="F53">
         <v>40</v>
@@ -2419,91 +2356,115 @@
       <c r="G53" t="s">
         <v>98</v>
       </c>
+      <c r="H53" t="s">
+        <v>31</v>
+      </c>
+      <c r="I53" t="s">
+        <v>44</v>
+      </c>
       <c r="J53" t="s">
-        <v>99</v>
+        <v>16</v>
       </c>
     </row>
     <row r="54" spans="1:10">
       <c r="A54" t="s">
-        <v>40</v>
+        <v>111</v>
       </c>
       <c r="B54" t="s">
-        <v>41</v>
+        <v>112</v>
       </c>
       <c r="D54">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E54" t="s">
+        <v>113</v>
+      </c>
+      <c r="F54">
         <v>50</v>
       </c>
-      <c r="F54">
-        <v>40</v>
-      </c>
       <c r="G54" t="s">
         <v>98</v>
       </c>
+      <c r="H54" t="s">
+        <v>31</v>
+      </c>
+      <c r="I54" t="s">
+        <v>54</v>
+      </c>
       <c r="J54" t="s">
-        <v>99</v>
+        <v>16</v>
       </c>
     </row>
     <row r="55" spans="1:10">
       <c r="A55" t="s">
-        <v>43</v>
+        <v>114</v>
       </c>
       <c r="B55" t="s">
-        <v>44</v>
+        <v>92</v>
       </c>
       <c r="D55">
         <v>1</v>
       </c>
       <c r="E55" t="s">
-        <v>45</v>
+        <v>105</v>
       </c>
       <c r="F55">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="G55" t="s">
         <v>98</v>
       </c>
+      <c r="H55" t="s">
+        <v>31</v>
+      </c>
+      <c r="I55" t="s">
+        <v>50</v>
+      </c>
       <c r="J55" t="s">
-        <v>99</v>
+        <v>16</v>
       </c>
     </row>
     <row r="56" spans="1:10">
       <c r="A56" t="s">
+        <v>32</v>
+      </c>
+      <c r="B56" t="s">
+        <v>33</v>
+      </c>
+      <c r="D56">
+        <v>3</v>
+      </c>
+      <c r="E56" t="s">
         <v>43</v>
       </c>
-      <c r="B56" t="s">
-        <v>44</v>
-      </c>
-      <c r="D56">
-        <v>2</v>
-      </c>
-      <c r="E56" t="s">
-        <v>78</v>
-      </c>
       <c r="F56">
-        <v>40</v>
+        <v>100</v>
       </c>
       <c r="G56" t="s">
         <v>98</v>
       </c>
+      <c r="H56" t="s">
+        <v>64</v>
+      </c>
+      <c r="I56" t="s">
+        <v>25</v>
+      </c>
       <c r="J56" t="s">
-        <v>99</v>
+        <v>16</v>
       </c>
     </row>
     <row r="57" spans="1:10">
       <c r="A57" t="s">
-        <v>43</v>
+        <v>22</v>
       </c>
       <c r="B57" t="s">
-        <v>44</v>
+        <v>23</v>
       </c>
       <c r="D57">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E57" t="s">
-        <v>78</v>
+        <v>108</v>
       </c>
       <c r="F57">
         <v>40</v>
@@ -2511,22 +2472,28 @@
       <c r="G57" t="s">
         <v>98</v>
       </c>
+      <c r="H57" t="s">
+        <v>64</v>
+      </c>
+      <c r="I57" t="s">
+        <v>21</v>
+      </c>
       <c r="J57" t="s">
-        <v>99</v>
+        <v>16</v>
       </c>
     </row>
     <row r="58" spans="1:10">
       <c r="A58" t="s">
-        <v>22</v>
+        <v>115</v>
       </c>
       <c r="B58" t="s">
-        <v>23</v>
+        <v>48</v>
       </c>
       <c r="D58">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E58" t="s">
-        <v>100</v>
+        <v>75</v>
       </c>
       <c r="F58">
         <v>40</v>
@@ -2534,22 +2501,28 @@
       <c r="G58" t="s">
         <v>98</v>
       </c>
+      <c r="H58" t="s">
+        <v>64</v>
+      </c>
+      <c r="I58" t="s">
+        <v>27</v>
+      </c>
       <c r="J58" t="s">
-        <v>99</v>
+        <v>16</v>
       </c>
     </row>
     <row r="59" spans="1:10">
       <c r="A59" t="s">
-        <v>22</v>
+        <v>91</v>
       </c>
       <c r="B59" t="s">
-        <v>23</v>
+        <v>92</v>
       </c>
       <c r="D59">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E59" t="s">
-        <v>100</v>
+        <v>116</v>
       </c>
       <c r="F59">
         <v>40</v>
@@ -2557,91 +2530,115 @@
       <c r="G59" t="s">
         <v>98</v>
       </c>
+      <c r="H59" t="s">
+        <v>64</v>
+      </c>
+      <c r="I59" t="s">
+        <v>44</v>
+      </c>
       <c r="J59" t="s">
-        <v>99</v>
+        <v>16</v>
       </c>
     </row>
     <row r="60" spans="1:10">
       <c r="A60" t="s">
-        <v>102</v>
+        <v>117</v>
       </c>
       <c r="B60" t="s">
-        <v>49</v>
+        <v>118</v>
       </c>
       <c r="D60">
         <v>1</v>
       </c>
       <c r="E60" t="s">
-        <v>75</v>
+        <v>119</v>
       </c>
       <c r="F60">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="G60" t="s">
         <v>98</v>
       </c>
+      <c r="H60" t="s">
+        <v>64</v>
+      </c>
+      <c r="I60" t="s">
+        <v>54</v>
+      </c>
       <c r="J60" t="s">
-        <v>99</v>
+        <v>16</v>
       </c>
     </row>
     <row r="61" spans="1:10">
       <c r="A61" t="s">
-        <v>48</v>
+        <v>120</v>
       </c>
       <c r="B61" t="s">
-        <v>49</v>
+        <v>107</v>
       </c>
       <c r="D61">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E61" t="s">
-        <v>19</v>
+        <v>121</v>
       </c>
       <c r="F61">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="G61" t="s">
         <v>98</v>
       </c>
+      <c r="H61" t="s">
+        <v>64</v>
+      </c>
+      <c r="I61" t="s">
+        <v>50</v>
+      </c>
       <c r="J61" t="s">
-        <v>99</v>
+        <v>16</v>
       </c>
     </row>
     <row r="62" spans="1:10">
       <c r="A62" t="s">
-        <v>91</v>
+        <v>32</v>
       </c>
       <c r="B62" t="s">
-        <v>92</v>
+        <v>33</v>
       </c>
       <c r="D62">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E62" t="s">
-        <v>19</v>
+        <v>43</v>
       </c>
       <c r="F62">
-        <v>40</v>
+        <v>100</v>
       </c>
       <c r="G62" t="s">
         <v>98</v>
       </c>
+      <c r="H62" t="s">
+        <v>72</v>
+      </c>
+      <c r="I62" t="s">
+        <v>25</v>
+      </c>
       <c r="J62" t="s">
-        <v>99</v>
+        <v>16</v>
       </c>
     </row>
     <row r="63" spans="1:10">
       <c r="A63" t="s">
-        <v>91</v>
+        <v>38</v>
       </c>
       <c r="B63" t="s">
-        <v>92</v>
+        <v>39</v>
       </c>
       <c r="D63">
         <v>2</v>
       </c>
       <c r="E63" t="s">
-        <v>103</v>
+        <v>49</v>
       </c>
       <c r="F63">
         <v>40</v>
@@ -2649,22 +2646,28 @@
       <c r="G63" t="s">
         <v>98</v>
       </c>
+      <c r="H63" t="s">
+        <v>72</v>
+      </c>
+      <c r="I63" t="s">
+        <v>21</v>
+      </c>
       <c r="J63" t="s">
-        <v>99</v>
+        <v>16</v>
       </c>
     </row>
     <row r="64" spans="1:10">
       <c r="A64" t="s">
-        <v>104</v>
+        <v>41</v>
       </c>
       <c r="B64" t="s">
-        <v>105</v>
+        <v>42</v>
       </c>
       <c r="D64">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E64" t="s">
-        <v>19</v>
+        <v>78</v>
       </c>
       <c r="F64">
         <v>40</v>
@@ -2672,16 +2675,22 @@
       <c r="G64" t="s">
         <v>98</v>
       </c>
+      <c r="H64" t="s">
+        <v>72</v>
+      </c>
+      <c r="I64" t="s">
+        <v>27</v>
+      </c>
       <c r="J64" t="s">
-        <v>99</v>
+        <v>16</v>
       </c>
     </row>
     <row r="65" spans="1:10">
       <c r="A65" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="B65" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="D65">
         <v>3</v>
@@ -2695,68 +2704,89 @@
       <c r="G65" t="s">
         <v>98</v>
       </c>
+      <c r="H65" t="s">
+        <v>72</v>
+      </c>
+      <c r="I65" t="s">
+        <v>44</v>
+      </c>
       <c r="J65" t="s">
-        <v>99</v>
+        <v>16</v>
       </c>
     </row>
     <row r="66" spans="1:10">
       <c r="A66" t="s">
-        <v>26</v>
+        <v>76</v>
       </c>
       <c r="B66" t="s">
-        <v>11</v>
+        <v>77</v>
       </c>
       <c r="D66">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E66" t="s">
-        <v>106</v>
+        <v>122</v>
       </c>
       <c r="F66">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="G66" t="s">
         <v>98</v>
       </c>
+      <c r="H66" t="s">
+        <v>72</v>
+      </c>
+      <c r="I66" t="s">
+        <v>54</v>
+      </c>
       <c r="J66" t="s">
-        <v>99</v>
+        <v>16</v>
       </c>
     </row>
     <row r="67" spans="1:10">
       <c r="A67" t="s">
-        <v>26</v>
+        <v>123</v>
       </c>
       <c r="B67" t="s">
-        <v>11</v>
+        <v>124</v>
       </c>
       <c r="D67">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E67" t="s">
-        <v>106</v>
+        <v>125</v>
       </c>
       <c r="F67">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="G67" t="s">
         <v>98</v>
       </c>
+      <c r="H67" t="s">
+        <v>72</v>
+      </c>
+      <c r="I67" t="s">
+        <v>50</v>
+      </c>
       <c r="J67" t="s">
-        <v>99</v>
+        <v>16</v>
       </c>
     </row>
     <row r="68" spans="1:10">
       <c r="A68" t="s">
-        <v>107</v>
+        <v>93</v>
       </c>
       <c r="B68" t="s">
-        <v>108</v>
+        <v>126</v>
+      </c>
+      <c r="C68" t="s">
+        <v>127</v>
       </c>
       <c r="D68">
         <v>1</v>
       </c>
       <c r="E68" t="s">
-        <v>109</v>
+        <v>128</v>
       </c>
       <c r="F68">
         <v>50</v>
@@ -2764,68 +2794,86 @@
       <c r="G68" t="s">
         <v>98</v>
       </c>
+      <c r="H68" t="s">
+        <v>72</v>
+      </c>
+      <c r="I68" t="s">
+        <v>62</v>
+      </c>
       <c r="J68" t="s">
-        <v>99</v>
+        <v>16</v>
       </c>
     </row>
     <row r="69" spans="1:10">
       <c r="A69" t="s">
-        <v>55</v>
+        <v>129</v>
       </c>
       <c r="B69" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="D69">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E69" t="s">
-        <v>19</v>
+        <v>130</v>
       </c>
       <c r="F69">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="G69" t="s">
         <v>98</v>
       </c>
+      <c r="H69" t="s">
+        <v>72</v>
+      </c>
+      <c r="I69" t="s">
+        <v>15</v>
+      </c>
       <c r="J69" t="s">
-        <v>99</v>
+        <v>16</v>
       </c>
     </row>
     <row r="70" spans="1:10">
       <c r="A70" t="s">
-        <v>55</v>
+        <v>86</v>
       </c>
       <c r="B70" t="s">
-        <v>56</v>
+        <v>87</v>
       </c>
       <c r="D70">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E70" t="s">
         <v>19</v>
       </c>
       <c r="F70">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="G70" t="s">
         <v>98</v>
       </c>
+      <c r="H70" t="s">
+        <v>88</v>
+      </c>
+      <c r="I70" t="s">
+        <v>21</v>
+      </c>
       <c r="J70" t="s">
-        <v>99</v>
+        <v>16</v>
       </c>
     </row>
     <row r="71" spans="1:10">
       <c r="A71" t="s">
-        <v>66</v>
+        <v>86</v>
       </c>
       <c r="B71" t="s">
-        <v>67</v>
+        <v>87</v>
       </c>
       <c r="D71">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E71" t="s">
-        <v>110</v>
+        <v>19</v>
       </c>
       <c r="F71">
         <v>40</v>
@@ -2833,39 +2881,51 @@
       <c r="G71" t="s">
         <v>98</v>
       </c>
+      <c r="H71" t="s">
+        <v>88</v>
+      </c>
+      <c r="I71" t="s">
+        <v>25</v>
+      </c>
       <c r="J71" t="s">
-        <v>99</v>
+        <v>16</v>
       </c>
     </row>
     <row r="72" spans="1:10">
       <c r="A72" t="s">
-        <v>76</v>
+        <v>35</v>
       </c>
       <c r="B72" t="s">
-        <v>77</v>
+        <v>36</v>
       </c>
       <c r="D72">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E72" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="F72">
-        <v>50</v>
+        <v>80</v>
       </c>
       <c r="G72" t="s">
         <v>98</v>
       </c>
+      <c r="H72" t="s">
+        <v>88</v>
+      </c>
+      <c r="I72" t="s">
+        <v>15</v>
+      </c>
       <c r="J72" t="s">
-        <v>99</v>
+        <v>16</v>
       </c>
     </row>
     <row r="73" spans="1:10">
       <c r="A73" t="s">
-        <v>112</v>
+        <v>89</v>
       </c>
       <c r="B73" t="s">
-        <v>113</v>
+        <v>90</v>
       </c>
       <c r="D73">
         <v>1</v>
@@ -2874,119 +2934,149 @@
         <v>19</v>
       </c>
       <c r="F73">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="G73" t="s">
         <v>98</v>
       </c>
+      <c r="H73" t="s">
+        <v>88</v>
+      </c>
+      <c r="I73" t="s">
+        <v>27</v>
+      </c>
       <c r="J73" t="s">
-        <v>99</v>
+        <v>16</v>
       </c>
     </row>
     <row r="74" spans="1:10">
       <c r="A74" t="s">
-        <v>112</v>
+        <v>89</v>
       </c>
       <c r="B74" t="s">
-        <v>113</v>
+        <v>90</v>
       </c>
       <c r="D74">
         <v>2</v>
       </c>
       <c r="E74" t="s">
-        <v>78</v>
+        <v>19</v>
       </c>
       <c r="F74">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="G74" t="s">
         <v>98</v>
       </c>
+      <c r="H74" t="s">
+        <v>88</v>
+      </c>
+      <c r="I74" t="s">
+        <v>44</v>
+      </c>
       <c r="J74" t="s">
-        <v>99</v>
+        <v>16</v>
       </c>
     </row>
     <row r="75" spans="1:10">
       <c r="A75" t="s">
-        <v>114</v>
+        <v>89</v>
       </c>
       <c r="B75" t="s">
-        <v>115</v>
+        <v>90</v>
       </c>
       <c r="D75">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E75" t="s">
-        <v>116</v>
+        <v>19</v>
       </c>
       <c r="F75">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="G75" t="s">
         <v>98</v>
       </c>
+      <c r="H75" t="s">
+        <v>88</v>
+      </c>
+      <c r="I75" t="s">
+        <v>46</v>
+      </c>
       <c r="J75" t="s">
-        <v>99</v>
+        <v>16</v>
       </c>
     </row>
     <row r="76" spans="1:10">
       <c r="A76" t="s">
-        <v>117</v>
+        <v>47</v>
       </c>
       <c r="B76" t="s">
-        <v>118</v>
+        <v>48</v>
       </c>
       <c r="D76">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E76" t="s">
-        <v>119</v>
+        <v>19</v>
       </c>
       <c r="F76">
+        <v>40</v>
+      </c>
+      <c r="G76" t="s">
+        <v>98</v>
+      </c>
+      <c r="H76" t="s">
+        <v>88</v>
+      </c>
+      <c r="I76" t="s">
         <v>50</v>
       </c>
-      <c r="G76" t="s">
-        <v>98</v>
-      </c>
       <c r="J76" t="s">
-        <v>99</v>
+        <v>16</v>
       </c>
     </row>
     <row r="77" spans="1:10">
       <c r="A77" t="s">
-        <v>82</v>
+        <v>55</v>
       </c>
       <c r="B77" t="s">
-        <v>120</v>
+        <v>56</v>
       </c>
       <c r="D77">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E77" t="s">
-        <v>119</v>
+        <v>19</v>
       </c>
       <c r="F77">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="G77" t="s">
         <v>98</v>
       </c>
+      <c r="H77" t="s">
+        <v>88</v>
+      </c>
+      <c r="I77" t="s">
+        <v>58</v>
+      </c>
       <c r="J77" t="s">
-        <v>99</v>
+        <v>16</v>
       </c>
     </row>
     <row r="78" spans="1:10">
       <c r="A78" t="s">
-        <v>121</v>
+        <v>106</v>
       </c>
       <c r="B78" t="s">
-        <v>122</v>
+        <v>107</v>
       </c>
       <c r="D78">
         <v>1</v>
       </c>
       <c r="E78" t="s">
-        <v>123</v>
+        <v>19</v>
       </c>
       <c r="F78">
         <v>50</v>
@@ -2994,22 +3084,28 @@
       <c r="G78" t="s">
         <v>98</v>
       </c>
+      <c r="H78" t="s">
+        <v>88</v>
+      </c>
+      <c r="I78" t="s">
+        <v>54</v>
+      </c>
       <c r="J78" t="s">
-        <v>99</v>
+        <v>16</v>
       </c>
     </row>
     <row r="79" spans="1:10">
       <c r="A79" t="s">
-        <v>124</v>
+        <v>131</v>
       </c>
       <c r="B79" t="s">
-        <v>125</v>
+        <v>132</v>
       </c>
       <c r="D79">
         <v>1</v>
       </c>
       <c r="E79" t="s">
-        <v>126</v>
+        <v>133</v>
       </c>
       <c r="F79">
         <v>50</v>
@@ -3017,94 +3113,115 @@
       <c r="G79" t="s">
         <v>98</v>
       </c>
+      <c r="H79" t="s">
+        <v>88</v>
+      </c>
+      <c r="I79" t="s">
+        <v>62</v>
+      </c>
       <c r="J79" t="s">
-        <v>99</v>
+        <v>16</v>
       </c>
     </row>
     <row r="80" spans="1:10">
       <c r="A80" t="s">
-        <v>93</v>
+        <v>68</v>
       </c>
       <c r="B80" t="s">
-        <v>127</v>
-      </c>
-      <c r="C80" t="s">
-        <v>128</v>
+        <v>69</v>
       </c>
       <c r="D80">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E80" t="s">
-        <v>129</v>
+        <v>19</v>
       </c>
       <c r="F80">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="G80" t="s">
         <v>98</v>
       </c>
+      <c r="H80" t="s">
+        <v>88</v>
+      </c>
+      <c r="I80" t="s">
+        <v>71</v>
+      </c>
       <c r="J80" t="s">
-        <v>99</v>
+        <v>16</v>
       </c>
     </row>
     <row r="81" spans="1:10">
       <c r="A81" t="s">
-        <v>130</v>
+        <v>89</v>
       </c>
       <c r="B81" t="s">
-        <v>131</v>
+        <v>90</v>
       </c>
       <c r="D81">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E81" t="s">
-        <v>132</v>
+        <v>19</v>
       </c>
       <c r="F81">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="G81" t="s">
         <v>98</v>
       </c>
+      <c r="H81" t="s">
+        <v>97</v>
+      </c>
+      <c r="I81" t="s">
+        <v>21</v>
+      </c>
       <c r="J81" t="s">
-        <v>99</v>
+        <v>16</v>
       </c>
     </row>
     <row r="82" spans="1:10">
       <c r="A82" t="s">
-        <v>133</v>
+        <v>55</v>
       </c>
       <c r="B82" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="D82">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E82" t="s">
-        <v>134</v>
+        <v>19</v>
       </c>
       <c r="F82">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="G82" t="s">
         <v>98</v>
       </c>
+      <c r="H82" t="s">
+        <v>97</v>
+      </c>
+      <c r="I82" t="s">
+        <v>25</v>
+      </c>
       <c r="J82" t="s">
-        <v>99</v>
+        <v>16</v>
       </c>
     </row>
     <row r="83" spans="1:10">
       <c r="A83" t="s">
-        <v>133</v>
+        <v>82</v>
       </c>
       <c r="B83" t="s">
-        <v>49</v>
+        <v>134</v>
       </c>
       <c r="D83">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E83" t="s">
-        <v>19</v>
+        <v>125</v>
       </c>
       <c r="F83">
         <v>50</v>
@@ -3112,8 +3229,14 @@
       <c r="G83" t="s">
         <v>98</v>
       </c>
+      <c r="H83" t="s">
+        <v>97</v>
+      </c>
+      <c r="I83" t="s">
+        <v>54</v>
+      </c>
       <c r="J83" t="s">
-        <v>99</v>
+        <v>16</v>
       </c>
     </row>
     <row r="84" spans="1:10">
@@ -3121,13 +3244,13 @@
         <v>135</v>
       </c>
       <c r="B84" t="s">
-        <v>92</v>
+        <v>136</v>
       </c>
       <c r="D84">
         <v>1</v>
       </c>
       <c r="E84" t="s">
-        <v>110</v>
+        <v>137</v>
       </c>
       <c r="F84">
         <v>50</v>
@@ -3135,42 +3258,48 @@
       <c r="G84" t="s">
         <v>98</v>
       </c>
+      <c r="H84" t="s">
+        <v>97</v>
+      </c>
+      <c r="I84" t="s">
+        <v>44</v>
+      </c>
       <c r="J84" t="s">
-        <v>99</v>
+        <v>16</v>
       </c>
     </row>
     <row r="85" spans="1:10">
       <c r="A85" t="s">
-        <v>136</v>
+        <v>35</v>
       </c>
       <c r="B85" t="s">
-        <v>113</v>
+        <v>36</v>
       </c>
       <c r="D85">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E85" t="s">
-        <v>137</v>
+        <v>19</v>
       </c>
       <c r="F85">
-        <v>50</v>
+        <v>80</v>
       </c>
       <c r="G85" t="s">
         <v>98</v>
       </c>
       <c r="J85" t="s">
-        <v>99</v>
+        <v>138</v>
       </c>
     </row>
     <row r="86" spans="1:10">
       <c r="A86" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
       <c r="B86" t="s">
-        <v>139</v>
+        <v>48</v>
       </c>
       <c r="D86">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E86" t="s">
         <v>19</v>
@@ -3182,21 +3311,21 @@
         <v>98</v>
       </c>
       <c r="J86" t="s">
-        <v>99</v>
+        <v>138</v>
       </c>
     </row>
     <row r="87" spans="1:10">
       <c r="A87" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B87" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D87">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E87" t="s">
-        <v>119</v>
+        <v>19</v>
       </c>
       <c r="F87">
         <v>50</v>
@@ -3205,30 +3334,30 @@
         <v>98</v>
       </c>
       <c r="J87" t="s">
-        <v>99</v>
+        <v>138</v>
       </c>
     </row>
     <row r="88" spans="1:10">
       <c r="A88" t="s">
-        <v>69</v>
+        <v>139</v>
       </c>
       <c r="B88" t="s">
-        <v>70</v>
+        <v>140</v>
       </c>
       <c r="D88">
         <v>2</v>
       </c>
       <c r="E88" t="s">
-        <v>19</v>
+        <v>125</v>
       </c>
       <c r="F88">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="G88" t="s">
         <v>98</v>
       </c>
       <c r="J88" t="s">
-        <v>99</v>
+        <v>138</v>
       </c>
     </row>
     <row r="89" spans="1:10">
@@ -3236,16 +3365,16 @@
         <v>93</v>
       </c>
       <c r="B89" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C89" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D89">
         <v>1</v>
       </c>
       <c r="E89" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="F89">
         <v>50</v>
@@ -3254,7 +3383,7 @@
         <v>20</v>
       </c>
       <c r="J89" t="s">
-        <v>99</v>
+        <v>138</v>
       </c>
     </row>
   </sheetData>
@@ -3264,7 +3393,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D52"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3272,730 +3401,86 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B1" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C1" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D1" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B2" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="C2" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="D2" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
+        <v>151</v>
+      </c>
+      <c r="B3" t="s">
+        <v>148</v>
+      </c>
+      <c r="C3" t="s">
+        <v>149</v>
+      </c>
+      <c r="D3" t="s">
         <v>150</v>
-      </c>
-      <c r="B3" t="s">
-        <v>149</v>
-      </c>
-      <c r="C3" t="s">
-        <v>151</v>
-      </c>
-      <c r="D3" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B4" t="s">
+        <v>148</v>
+      </c>
+      <c r="C4" t="s">
         <v>149</v>
       </c>
-      <c r="C4" t="s">
-        <v>151</v>
-      </c>
       <c r="D4" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B5" t="s">
+        <v>148</v>
+      </c>
+      <c r="C5" t="s">
         <v>149</v>
       </c>
-      <c r="C5" t="s">
-        <v>151</v>
-      </c>
       <c r="D5" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B6" t="s">
+        <v>148</v>
+      </c>
+      <c r="C6" t="s">
         <v>149</v>
       </c>
-      <c r="C6" t="s">
-        <v>151</v>
-      </c>
       <c r="D6" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" t="s">
-        <v>156</v>
-      </c>
-      <c r="B7" t="s">
-        <v>149</v>
-      </c>
-      <c r="C7" t="s">
-        <v>151</v>
-      </c>
-      <c r="D7" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8" t="s">
-        <v>157</v>
-      </c>
-      <c r="B8" t="s">
-        <v>149</v>
-      </c>
-      <c r="C8" t="s">
-        <v>151</v>
-      </c>
-      <c r="D8" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9" t="s">
-        <v>158</v>
-      </c>
-      <c r="B9" t="s">
-        <v>147</v>
-      </c>
-      <c r="C9" t="s">
-        <v>148</v>
-      </c>
-      <c r="D9" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" t="s">
-        <v>159</v>
-      </c>
-      <c r="B10" t="s">
-        <v>147</v>
-      </c>
-      <c r="C10" t="s">
-        <v>148</v>
-      </c>
-      <c r="D10" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11" t="s">
-        <v>160</v>
-      </c>
-      <c r="B11" t="s">
-        <v>147</v>
-      </c>
-      <c r="C11" t="s">
-        <v>148</v>
-      </c>
-      <c r="D11" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12" t="s">
-        <v>161</v>
-      </c>
-      <c r="B12" t="s">
-        <v>147</v>
-      </c>
-      <c r="C12" t="s">
-        <v>148</v>
-      </c>
-      <c r="D12" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="A13" t="s">
-        <v>162</v>
-      </c>
-      <c r="B13" t="s">
-        <v>147</v>
-      </c>
-      <c r="C13" t="s">
-        <v>148</v>
-      </c>
-      <c r="D13" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="A14" t="s">
-        <v>163</v>
-      </c>
-      <c r="B14" t="s">
-        <v>147</v>
-      </c>
-      <c r="C14" t="s">
-        <v>148</v>
-      </c>
-      <c r="D14" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
-      <c r="A15" t="s">
-        <v>164</v>
-      </c>
-      <c r="B15" t="s">
-        <v>147</v>
-      </c>
-      <c r="C15" t="s">
-        <v>148</v>
-      </c>
-      <c r="D15" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
-      <c r="A16" t="s">
-        <v>165</v>
-      </c>
-      <c r="B16" t="s">
-        <v>147</v>
-      </c>
-      <c r="C16" t="s">
-        <v>148</v>
-      </c>
-      <c r="D16" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
-      <c r="A17" t="s">
-        <v>166</v>
-      </c>
-      <c r="B17" t="s">
-        <v>147</v>
-      </c>
-      <c r="C17" t="s">
-        <v>148</v>
-      </c>
-      <c r="D17" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
-      <c r="A18" t="s">
-        <v>167</v>
-      </c>
-      <c r="B18" t="s">
-        <v>147</v>
-      </c>
-      <c r="C18" t="s">
-        <v>148</v>
-      </c>
-      <c r="D18" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4">
-      <c r="A19" t="s">
-        <v>168</v>
-      </c>
-      <c r="B19" t="s">
-        <v>147</v>
-      </c>
-      <c r="C19" t="s">
-        <v>148</v>
-      </c>
-      <c r="D19" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4">
-      <c r="A20" t="s">
-        <v>169</v>
-      </c>
-      <c r="B20" t="s">
-        <v>147</v>
-      </c>
-      <c r="C20" t="s">
-        <v>148</v>
-      </c>
-      <c r="D20" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4">
-      <c r="A21" t="s">
-        <v>170</v>
-      </c>
-      <c r="B21" t="s">
-        <v>147</v>
-      </c>
-      <c r="C21" t="s">
-        <v>148</v>
-      </c>
-      <c r="D21" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4">
-      <c r="A22" t="s">
-        <v>171</v>
-      </c>
-      <c r="B22" t="s">
-        <v>147</v>
-      </c>
-      <c r="C22" t="s">
-        <v>148</v>
-      </c>
-      <c r="D22" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4">
-      <c r="A23" t="s">
-        <v>172</v>
-      </c>
-      <c r="B23" t="s">
-        <v>147</v>
-      </c>
-      <c r="C23" t="s">
-        <v>148</v>
-      </c>
-      <c r="D23" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4">
-      <c r="A24" t="s">
-        <v>173</v>
-      </c>
-      <c r="B24" t="s">
-        <v>147</v>
-      </c>
-      <c r="C24" t="s">
-        <v>148</v>
-      </c>
-      <c r="D24" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4">
-      <c r="A25" t="s">
-        <v>174</v>
-      </c>
-      <c r="B25" t="s">
-        <v>147</v>
-      </c>
-      <c r="C25" t="s">
-        <v>148</v>
-      </c>
-      <c r="D25" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4">
-      <c r="A26" t="s">
-        <v>175</v>
-      </c>
-      <c r="B26" t="s">
-        <v>147</v>
-      </c>
-      <c r="C26" t="s">
-        <v>148</v>
-      </c>
-      <c r="D26" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4">
-      <c r="A27" t="s">
-        <v>176</v>
-      </c>
-      <c r="B27" t="s">
-        <v>147</v>
-      </c>
-      <c r="C27" t="s">
-        <v>148</v>
-      </c>
-      <c r="D27" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4">
-      <c r="A28" t="s">
-        <v>177</v>
-      </c>
-      <c r="B28" t="s">
-        <v>147</v>
-      </c>
-      <c r="C28" t="s">
-        <v>148</v>
-      </c>
-      <c r="D28" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4">
-      <c r="A29" t="s">
-        <v>178</v>
-      </c>
-      <c r="B29" t="s">
-        <v>147</v>
-      </c>
-      <c r="C29" t="s">
-        <v>148</v>
-      </c>
-      <c r="D29" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4">
-      <c r="A30" t="s">
-        <v>179</v>
-      </c>
-      <c r="B30" t="s">
-        <v>149</v>
-      </c>
-      <c r="C30" t="s">
-        <v>180</v>
-      </c>
-      <c r="D30" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4">
-      <c r="A31" t="s">
-        <v>181</v>
-      </c>
-      <c r="B31" t="s">
-        <v>182</v>
-      </c>
-      <c r="C31" t="s">
-        <v>147</v>
-      </c>
-      <c r="D31" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4">
-      <c r="A32" t="s">
-        <v>183</v>
-      </c>
-      <c r="B32" t="s">
-        <v>182</v>
-      </c>
-      <c r="C32" t="s">
-        <v>147</v>
-      </c>
-      <c r="D32" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4">
-      <c r="A33" t="s">
-        <v>184</v>
-      </c>
-      <c r="B33" t="s">
-        <v>147</v>
-      </c>
-      <c r="C33" t="s">
-        <v>148</v>
-      </c>
-      <c r="D33" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4">
-      <c r="A34" t="s">
-        <v>185</v>
-      </c>
-      <c r="B34" t="s">
-        <v>149</v>
-      </c>
-      <c r="C34" t="s">
-        <v>180</v>
-      </c>
-      <c r="D34" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4">
-      <c r="A35" t="s">
-        <v>186</v>
-      </c>
-      <c r="B35" t="s">
-        <v>149</v>
-      </c>
-      <c r="C35" t="s">
-        <v>180</v>
-      </c>
-      <c r="D35" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4">
-      <c r="A36" t="s">
-        <v>187</v>
-      </c>
-      <c r="B36" t="s">
-        <v>149</v>
-      </c>
-      <c r="C36" t="s">
-        <v>180</v>
-      </c>
-      <c r="D36" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4">
-      <c r="A37" t="s">
-        <v>188</v>
-      </c>
-      <c r="B37" t="s">
-        <v>149</v>
-      </c>
-      <c r="C37" t="s">
-        <v>180</v>
-      </c>
-      <c r="D37" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4">
-      <c r="A38" t="s">
-        <v>189</v>
-      </c>
-      <c r="B38" t="s">
-        <v>149</v>
-      </c>
-      <c r="C38" t="s">
-        <v>180</v>
-      </c>
-      <c r="D38" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4">
-      <c r="A39" t="s">
-        <v>190</v>
-      </c>
-      <c r="B39" t="s">
-        <v>149</v>
-      </c>
-      <c r="C39" t="s">
-        <v>180</v>
-      </c>
-      <c r="D39" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4">
-      <c r="A40" t="s">
-        <v>191</v>
-      </c>
-      <c r="B40" t="s">
-        <v>149</v>
-      </c>
-      <c r="C40" t="s">
-        <v>180</v>
-      </c>
-      <c r="D40" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4">
-      <c r="A41" t="s">
-        <v>192</v>
-      </c>
-      <c r="B41" t="s">
-        <v>149</v>
-      </c>
-      <c r="C41" t="s">
-        <v>180</v>
-      </c>
-      <c r="D41" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4">
-      <c r="A42" t="s">
-        <v>193</v>
-      </c>
-      <c r="B42" t="s">
-        <v>149</v>
-      </c>
-      <c r="C42" t="s">
-        <v>180</v>
-      </c>
-      <c r="D42" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4">
-      <c r="A43" t="s">
-        <v>194</v>
-      </c>
-      <c r="B43" t="s">
-        <v>149</v>
-      </c>
-      <c r="C43" t="s">
-        <v>180</v>
-      </c>
-      <c r="D43" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4">
-      <c r="A44" t="s">
-        <v>195</v>
-      </c>
-      <c r="B44" t="s">
-        <v>149</v>
-      </c>
-      <c r="C44" t="s">
-        <v>180</v>
-      </c>
-      <c r="D44" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4">
-      <c r="A45" t="s">
-        <v>196</v>
-      </c>
-      <c r="B45" t="s">
-        <v>149</v>
-      </c>
-      <c r="C45" t="s">
-        <v>180</v>
-      </c>
-      <c r="D45" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4">
-      <c r="A46" t="s">
-        <v>197</v>
-      </c>
-      <c r="B46" t="s">
-        <v>149</v>
-      </c>
-      <c r="C46" t="s">
-        <v>180</v>
-      </c>
-      <c r="D46" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4">
-      <c r="A47" t="s">
-        <v>198</v>
-      </c>
-      <c r="B47" t="s">
-        <v>149</v>
-      </c>
-      <c r="C47" t="s">
-        <v>180</v>
-      </c>
-      <c r="D47" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4">
-      <c r="A48" t="s">
-        <v>199</v>
-      </c>
-      <c r="B48" t="s">
-        <v>149</v>
-      </c>
-      <c r="C48" t="s">
-        <v>180</v>
-      </c>
-      <c r="D48" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4">
-      <c r="A49" t="s">
-        <v>200</v>
-      </c>
-      <c r="B49" t="s">
-        <v>149</v>
-      </c>
-      <c r="C49" t="s">
-        <v>180</v>
-      </c>
-      <c r="D49" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4">
-      <c r="A50" t="s">
-        <v>201</v>
-      </c>
-      <c r="B50" t="s">
-        <v>147</v>
-      </c>
-      <c r="C50" t="s">
-        <v>148</v>
-      </c>
-      <c r="D50" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4">
-      <c r="A51" t="s">
-        <v>202</v>
-      </c>
-      <c r="B51" t="s">
-        <v>149</v>
-      </c>
-      <c r="C51" t="s">
-        <v>180</v>
-      </c>
-      <c r="D51" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4">
-      <c r="A52" t="s">
-        <v>203</v>
-      </c>
-      <c r="B52" t="s">
-        <v>149</v>
-      </c>
-      <c r="C52" t="s">
-        <v>180</v>
-      </c>
-      <c r="D52" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
   </sheetData>

</xml_diff>